<commit_message>
excel and test updates
</commit_message>
<xml_diff>
--- a/IT23818866_Assignment1 ITP .xlsx
+++ b/IT23818866_Assignment1 ITP .xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shena\Desktop\Assignment1 ITP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shena\Desktop\IT23818866\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5916"/>
   </bookViews>
   <sheets>
     <sheet name="Regenerated Test Cases with New" sheetId="1" r:id="rId1"/>
@@ -288,9 +288,6 @@
     <t xml:space="preserve"> Mixed Singlish + English · Simple sentence · S (≤30 characters) · Accuracy validation</t>
   </si>
   <si>
-    <t>Pos_Fun_0024</t>
-  </si>
-  <si>
     <t>Mixed English + Singlish</t>
   </si>
   <si>
@@ -300,9 +297,6 @@
     <t xml:space="preserve"> Mixed Singlish + English · Simple sentence · M (31–299 characters) · Accuracy validation</t>
   </si>
   <si>
-    <t>Pos_Fun_0025</t>
-  </si>
-  <si>
     <t>Currency format handling</t>
   </si>
   <si>
@@ -312,9 +306,6 @@
     <t xml:space="preserve"> Punctuation / numbers · Simple sentence · S (≤30 characters) · Accuracy validation</t>
   </si>
   <si>
-    <t>Pos_Fun_0026</t>
-  </si>
-  <si>
     <t>Units of measurement</t>
   </si>
   <si>
@@ -676,6 +667,15 @@
   </si>
   <si>
     <t xml:space="preserve"> රම්</t>
+  </si>
+  <si>
+    <t>Pos_Fun_0001</t>
+  </si>
+  <si>
+    <t>Pos_Fun_0002</t>
+  </si>
+  <si>
+    <t>Pos_Fun_0003</t>
   </si>
 </sst>
 </file>
@@ -972,8 +972,8 @@
   </sheetPr>
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -988,7 +988,7 @@
     <col min="9" max="9" width="88.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1019,7 +1019,7 @@
     </row>
     <row r="2" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>10</v>
@@ -1028,13 +1028,13 @@
         <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>12</v>
@@ -1048,7 +1048,7 @@
     </row>
     <row r="3" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>217</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>16</v>
@@ -1057,13 +1057,13 @@
         <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>12</v>
@@ -1077,7 +1077,7 @@
     </row>
     <row r="4" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>218</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>21</v>
@@ -1086,13 +1086,13 @@
         <v>17</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>12</v>
@@ -1106,22 +1106,22 @@
     </row>
     <row r="5" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>12</v>
@@ -1130,12 +1130,12 @@
         <v>26</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>28</v>
@@ -1144,13 +1144,13 @@
         <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>12</v>
@@ -1164,7 +1164,7 @@
     </row>
     <row r="7" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>32</v>
@@ -1173,13 +1173,13 @@
         <v>17</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>12</v>
@@ -1193,7 +1193,7 @@
     </row>
     <row r="8" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>36</v>
@@ -1202,13 +1202,13 @@
         <v>11</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>12</v>
@@ -1222,7 +1222,7 @@
     </row>
     <row r="9" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>40</v>
@@ -1231,13 +1231,13 @@
         <v>11</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>12</v>
@@ -1251,7 +1251,7 @@
     </row>
     <row r="10" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>44</v>
@@ -1260,13 +1260,13 @@
         <v>17</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>12</v>
@@ -1280,7 +1280,7 @@
     </row>
     <row r="11" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>48</v>
@@ -1289,13 +1289,13 @@
         <v>17</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>12</v>
@@ -1309,7 +1309,7 @@
     </row>
     <row r="12" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>52</v>
@@ -1318,13 +1318,13 @@
         <v>11</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>12</v>
@@ -1338,7 +1338,7 @@
     </row>
     <row r="13" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>56</v>
@@ -1347,13 +1347,13 @@
         <v>11</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>12</v>
@@ -1367,7 +1367,7 @@
     </row>
     <row r="14" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>59</v>
@@ -1376,13 +1376,13 @@
         <v>11</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>12</v>
@@ -1396,7 +1396,7 @@
     </row>
     <row r="15" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>63</v>
@@ -1405,13 +1405,13 @@
         <v>11</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>12</v>
@@ -1425,7 +1425,7 @@
     </row>
     <row r="16" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>66</v>
@@ -1434,13 +1434,13 @@
         <v>11</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>12</v>
@@ -1454,7 +1454,7 @@
     </row>
     <row r="17" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>70</v>
@@ -1463,13 +1463,13 @@
         <v>11</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>12</v>
@@ -1483,7 +1483,7 @@
     </row>
     <row r="18" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>74</v>
@@ -1492,13 +1492,13 @@
         <v>11</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>12</v>
@@ -1512,7 +1512,7 @@
     </row>
     <row r="19" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>78</v>
@@ -1521,13 +1521,13 @@
         <v>11</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>12</v>
@@ -1541,7 +1541,7 @@
     </row>
     <row r="20" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>82</v>
@@ -1550,13 +1550,13 @@
         <v>11</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>12</v>
@@ -1570,7 +1570,7 @@
     </row>
     <row r="21" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>86</v>
@@ -1579,13 +1579,13 @@
         <v>11</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>12</v>
@@ -1599,408 +1599,408 @@
     </row>
     <row r="22" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>90</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H22" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I22" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="I23" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="F25" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="1" t="s">
+      <c r="I25" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="F26" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="2" t="s">
+      <c r="G26" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="H26" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="I26" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="F27" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="2" t="s">
+      <c r="G27" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H27" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="I27" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H28" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="I28" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="F30" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" s="2" t="s">
+      <c r="G30" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H30" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>135</v>
-      </c>
       <c r="I30" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="I31" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E32" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="F32" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D32" s="2" t="s">
+      <c r="G32" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="I32" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I33" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E34" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="F34" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D34" s="2" t="s">
+      <c r="G34" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H34" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="I34" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>